<commit_message>
Completed design draft and documentation
</commit_message>
<xml_diff>
--- a/Mission_to_Mars/web_scraping_proj_reqs.xlsx
+++ b/Mission_to_Mars/web_scraping_proj_reqs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KDSharp\data-science\smu-bootcamp\web-scraping-challenge\Mission_to_Mars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE3E568-2A52-4CEB-9FD4-1956EC0A7BAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1309625-E71A-4EB5-903C-ADD7E2EF8161}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2628" yWindow="1752" windowWidth="16404" windowHeight="10620" xr2:uid="{CE5C240E-7DC8-42B1-ACAC-0529254F3C94}"/>
+    <workbookView xWindow="648" yWindow="504" windowWidth="20136" windowHeight="11880" xr2:uid="{CE5C240E-7DC8-42B1-ACAC-0529254F3C94}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
   <si>
     <t>Requirement</t>
   </si>
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>DataSource_element</t>
-  </si>
-  <si>
-    <t>variableName_tbd</t>
   </si>
   <si>
     <t>featured_image_url</t>
@@ -519,6 +516,15 @@
     <t>Use Splinter to navigate the sites when needed and BeautifulSoup to help find and parse out the necessary data.
 Use Pymongo for CRUD applications for your database. For this homework, you can simply overwrite the existing document each time the /scrape url is visited and new data is obtained.
 Use Bootstrap to structure your HTML template.</t>
+  </si>
+  <si>
+    <t>news_title</t>
+  </si>
+  <si>
+    <t>news_text</t>
+  </si>
+  <si>
+    <t>mars_facts_html</t>
   </si>
 </sst>
 </file>
@@ -839,26 +845,26 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1177,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98B75072-9A77-473E-AC62-ECE22FB85DF5}">
   <dimension ref="A2:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:F3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.6" customHeight="1"/>
@@ -1194,26 +1200,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="30.6" customHeight="1" thickBot="1">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="1:7" s="29" customFormat="1" ht="74.400000000000006" customHeight="1">
+      <c r="B3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:7" s="32" customFormat="1" ht="74.400000000000006" customHeight="1">
-      <c r="B3" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:7" ht="10.199999999999999" customHeight="1"/>
     <row r="5" spans="1:7" s="7" customFormat="1" ht="30.6" customHeight="1">
@@ -1221,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>0</v>
@@ -1241,13 +1247,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>10</v>
@@ -1260,7 +1266,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>3</v>
@@ -1279,7 +1285,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>30</v>
+        <v>84</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>18</v>
@@ -1293,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>19</v>
@@ -1304,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>13</v>
@@ -1328,7 +1334,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>17</v>
@@ -1339,7 +1345,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>20</v>
@@ -1355,7 +1361,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>24</v>
@@ -1371,7 +1377,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>25</v>
@@ -1389,7 +1395,7 @@
         <v>28</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="51" customHeight="1">
@@ -1397,22 +1403,22 @@
         <v>5</v>
       </c>
       <c r="C18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>41</v>
-      </c>
       <c r="F18" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G18" s="9"/>
     </row>
     <row r="19" spans="2:7" ht="30.6" customHeight="1">
       <c r="D19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F19" s="4"/>
     </row>
@@ -1421,14 +1427,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="14.4">
@@ -1436,13 +1442,13 @@
         <v>5.2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="28.8">
@@ -1450,10 +1456,10 @@
         <v>5.3</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="86.4">
@@ -1461,24 +1467,24 @@
         <v>5.4</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="2:7" s="6" customFormat="1" ht="67.2" customHeight="1">
       <c r="B24" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="D24" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
@@ -1489,10 +1495,10 @@
         <v>1</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E25" s="17"/>
       <c r="F25" s="16"/>
@@ -1504,10 +1510,10 @@
       </c>
       <c r="C26" s="18"/>
       <c r="D26" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
@@ -1517,10 +1523,10 @@
         <v>1.2</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="60.6" customHeight="1">
@@ -1528,15 +1534,15 @@
         <v>2</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E28" s="17"/>
       <c r="F28" s="16"/>
       <c r="G28" s="25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="67.2" customHeight="1">
@@ -1544,10 +1550,10 @@
         <v>2.1</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="30.6" customHeight="1">
@@ -1555,10 +1561,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30.6" customHeight="1">
@@ -1566,10 +1572,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="60.6" customHeight="1">
@@ -1577,10 +1583,10 @@
         <v>3</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" s="17"/>
       <c r="F32" s="16"/>
@@ -1588,13 +1594,13 @@
     </row>
     <row r="33" spans="2:7" ht="30.6" customHeight="1">
       <c r="B33" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E33" s="28"/>
       <c r="F33" s="27"/>
@@ -1605,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30.6" customHeight="1">
@@ -1613,7 +1619,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="30.6" customHeight="1">
@@ -1621,7 +1627,7 @@
         <v>3</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1636,8 +1642,9 @@
     <hyperlink ref="E10" r:id="rId2" xr:uid="{22191193-C870-4EA6-A69F-BFDD3DA920F5}"/>
     <hyperlink ref="E13" r:id="rId3" xr:uid="{522701E6-A37A-433E-B4B2-F8B15AF10E45}"/>
     <hyperlink ref="E16" r:id="rId4" xr:uid="{F7FBB0AD-D5F2-4300-90C9-1EFA7002D803}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{37654EAB-2596-476F-8921-DC99EC13D4BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>